<commit_message>
✨ feat(data): add column to data dict
</commit_message>
<xml_diff>
--- a/data/data_dictionary.xlsx
+++ b/data/data_dictionary.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juanp\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juanp\Downloads\Academic_Performance_Regression\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{616E1EA8-42F3-4705-B6E6-95A6C3D62FD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{318C541C-60B4-4BB6-AFB3-A73769D6DFAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="40">
-  <si>
-    <t>Variable</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="57">
   <si>
     <t>Tipo</t>
   </si>
@@ -140,13 +137,67 @@
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>ID_Alumno</t>
+  </si>
+  <si>
+    <t>Edad</t>
+  </si>
+  <si>
+    <t>Genero</t>
+  </si>
+  <si>
+    <t>Horas_Estudio</t>
+  </si>
+  <si>
+    <t>Redes_Sociales</t>
+  </si>
+  <si>
+    <t>Netflix</t>
+  </si>
+  <si>
+    <t>Trabajo</t>
+  </si>
+  <si>
+    <t>Asistencia</t>
+  </si>
+  <si>
+    <t>Horas_Sueño</t>
+  </si>
+  <si>
+    <t>Calidad_Dieta</t>
+  </si>
+  <si>
+    <t>Frecuencia_Ejercicio</t>
+  </si>
+  <si>
+    <t>Educacion_Parental</t>
+  </si>
+  <si>
+    <t>Calidad_Internet</t>
+  </si>
+  <si>
+    <t>Salud_Mental</t>
+  </si>
+  <si>
+    <t>Act_Extraescolar</t>
+  </si>
+  <si>
+    <t>Puntaje_Examen</t>
+  </si>
+  <si>
+    <t>Variables</t>
+  </si>
+  <si>
+    <t>Nombre Original</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -157,6 +208,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -274,15 +333,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -296,6 +349,19 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -601,309 +667,363 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.77734375" customWidth="1"/>
-    <col min="4" max="4" width="9.21875" customWidth="1"/>
-    <col min="5" max="5" width="56.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.77734375" customWidth="1"/>
+    <col min="5" max="5" width="9.21875" customWidth="1"/>
+    <col min="6" max="6" width="56.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="24.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:6" ht="24.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="D1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="F1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="11" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="C2" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C3" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E2" s="4" t="s">
+      <c r="D3" s="10">
+        <v>17</v>
+      </c>
+      <c r="E3" s="10">
+        <v>24</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="2">
+      <c r="C4" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="10">
+        <v>0</v>
+      </c>
+      <c r="E5" s="10">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="10">
+        <v>0</v>
+      </c>
+      <c r="E6" s="10">
+        <v>7.2</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="10">
+        <v>0</v>
+      </c>
+      <c r="E7" s="10">
+        <v>5.4</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="10">
+        <v>56</v>
+      </c>
+      <c r="E9" s="10">
+        <v>100</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="10">
+        <v>3.2</v>
+      </c>
+      <c r="E10" s="10">
+        <v>10</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="10">
+        <v>0</v>
+      </c>
+      <c r="E12" s="10">
+        <v>6</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="2">
-        <v>24</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="C15" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="2">
-        <v>0</v>
-      </c>
-      <c r="D5" s="2">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="2">
-        <v>0</v>
-      </c>
-      <c r="D6" s="2">
-        <v>7.2</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="D15" s="10">
+        <v>1</v>
+      </c>
+      <c r="E15" s="10">
         <v>10</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="2">
-        <v>0</v>
-      </c>
-      <c r="D7" s="2">
-        <v>5.4</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="1" t="s">
+      <c r="F15" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="2">
-        <v>56</v>
-      </c>
-      <c r="D9" s="2">
+      <c r="D17" s="3">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="E17" s="3">
         <v>100</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="2">
-        <v>3.2</v>
-      </c>
-      <c r="D10" s="2">
-        <v>10</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="2">
-        <v>0</v>
-      </c>
-      <c r="D12" s="2">
-        <v>6</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="2">
-        <v>1</v>
-      </c>
-      <c r="D15" s="2">
-        <v>10</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E16" s="4" t="s">
+      <c r="F17" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" s="7">
-        <v>18.399999999999999</v>
-      </c>
-      <c r="D17" s="7">
-        <v>100</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>38</v>
-      </c>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>